<commit_message>
se acomodaron cosas, se subio estado del excel.
</commit_message>
<xml_diff>
--- a/ProjectItems/Tareas iCatalog.xlsx
+++ b/ProjectItems/Tareas iCatalog.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="75" windowWidth="20115" windowHeight="7995"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="97">
   <si>
     <t>Tarea</t>
   </si>
@@ -301,13 +301,22 @@
   </si>
   <si>
     <t>Persona</t>
+  </si>
+  <si>
+    <t>Sebas/Pablo</t>
+  </si>
+  <si>
+    <t>pending</t>
+  </si>
+  <si>
+    <t>not assigned</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -324,7 +333,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -358,6 +367,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF66"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -399,7 +420,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -430,19 +451,22 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
+    <cellStyle name="Heading 2" xfId="1" builtinId="17"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Título 2" xfId="1" builtinId="17"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -460,7 +484,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -534,6 +558,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -568,6 +593,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -743,14 +769,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="45" customWidth="1"/>
     <col min="2" max="2" width="59" customWidth="1"/>
@@ -759,26 +785,26 @@
     <col min="7" max="7" width="12.7109375" style="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="11"/>
       <c r="B4" s="11"/>
     </row>
-    <row r="5" spans="1:7" ht="18" thickBot="1">
+    <row r="5" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="12" t="s">
         <v>0</v>
       </c>
@@ -797,11 +823,11 @@
       <c r="F5" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="G5" s="14" t="s">
+      <c r="G5" s="13" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" thickTop="1">
+    <row r="6" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
@@ -814,9 +840,11 @@
       <c r="F6" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="G6" s="16"/>
-    </row>
-    <row r="7" spans="1:7">
+      <c r="G6" s="17" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
@@ -829,9 +857,11 @@
       <c r="F7" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="G7" s="16"/>
-    </row>
-    <row r="8" spans="1:7">
+      <c r="G7" s="17" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>9</v>
       </c>
@@ -844,9 +874,11 @@
       <c r="F8" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="G8" s="16"/>
-    </row>
-    <row r="9" spans="1:7">
+      <c r="G8" s="17" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>11</v>
       </c>
@@ -859,9 +891,11 @@
       <c r="F9" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="G9" s="16"/>
-    </row>
-    <row r="10" spans="1:7">
+      <c r="G9" s="17" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>13</v>
       </c>
@@ -874,9 +908,11 @@
       <c r="F10" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="G10" s="16"/>
-    </row>
-    <row r="11" spans="1:7" ht="30">
+      <c r="G10" s="17" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>18</v>
       </c>
@@ -886,12 +922,14 @@
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
-      <c r="F11" s="17" t="s">
+      <c r="F11" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="G11" s="16"/>
-    </row>
-    <row r="12" spans="1:7">
+      <c r="G11" s="17" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>65</v>
       </c>
@@ -904,9 +942,11 @@
       <c r="F12" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="G12" s="16"/>
-    </row>
-    <row r="13" spans="1:7">
+      <c r="G12" s="17" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>16</v>
       </c>
@@ -919,9 +959,11 @@
       <c r="F13" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="G13" s="16"/>
-    </row>
-    <row r="14" spans="1:7">
+      <c r="G13" s="17" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>19</v>
       </c>
@@ -934,9 +976,11 @@
       <c r="F14" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="G14" s="16"/>
-    </row>
-    <row r="15" spans="1:7">
+      <c r="G14" s="17" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>67</v>
       </c>
@@ -949,9 +993,11 @@
       <c r="F15" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="G15" s="16"/>
-    </row>
-    <row r="16" spans="1:7">
+      <c r="G15" s="17" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>21</v>
       </c>
@@ -964,9 +1010,11 @@
       <c r="F16" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="G16" s="16"/>
-    </row>
-    <row r="17" spans="1:7" ht="30">
+      <c r="G16" s="17" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>23</v>
       </c>
@@ -976,12 +1024,14 @@
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18" t="s">
+      <c r="F17" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="G17" s="17" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="30">
+    <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>35</v>
       </c>
@@ -991,12 +1041,14 @@
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18" t="s">
+      <c r="F18" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="G18" s="17" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>74</v>
       </c>
@@ -1006,12 +1058,14 @@
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18" t="s">
+      <c r="F19" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="G19" s="17" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>69</v>
       </c>
@@ -1021,12 +1075,14 @@
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18" t="s">
+      <c r="F20" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="G20" s="17" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="30">
+    <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>47</v>
       </c>
@@ -1036,12 +1092,14 @@
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18" t="s">
+      <c r="F21" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="G21" s="17" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>75</v>
       </c>
@@ -1051,12 +1109,14 @@
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="18" t="s">
+      <c r="F22" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="G22" s="17" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>77</v>
       </c>
@@ -1066,12 +1126,14 @@
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18" t="s">
+      <c r="F23" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="G23" s="17" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="30">
+    <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>81</v>
       </c>
@@ -1081,10 +1143,12 @@
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="18"/>
-    </row>
-    <row r="25" spans="1:7" ht="30">
+      <c r="F24" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="G24" s="17"/>
+    </row>
+    <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>71</v>
       </c>
@@ -1094,10 +1158,12 @@
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
-      <c r="F25" s="18"/>
-      <c r="G25" s="18"/>
-    </row>
-    <row r="26" spans="1:7" ht="30">
+      <c r="F25" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="G25" s="17"/>
+    </row>
+    <row r="26" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>26</v>
       </c>
@@ -1107,12 +1173,14 @@
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="18" t="s">
+      <c r="F26" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="G26" s="17" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="30">
+    <row r="27" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>28</v>
       </c>
@@ -1122,12 +1190,14 @@
       <c r="C27" s="7"/>
       <c r="D27" s="7"/>
       <c r="E27" s="7"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18" t="s">
+      <c r="F27" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="G27" s="17" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="30">
+    <row r="28" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
         <v>38</v>
       </c>
@@ -1137,12 +1207,14 @@
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
       <c r="E28" s="7"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="18" t="s">
+      <c r="F28" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="G28" s="17" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
         <v>31</v>
       </c>
@@ -1152,12 +1224,14 @@
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
       <c r="E29" s="7"/>
-      <c r="F29" s="18"/>
-      <c r="G29" s="18" t="s">
+      <c r="F29" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="G29" s="17" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="45.75" customHeight="1">
+    <row r="30" spans="1:7" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
         <v>43</v>
       </c>
@@ -1167,12 +1241,14 @@
       <c r="C30" s="7"/>
       <c r="D30" s="7"/>
       <c r="E30" s="7"/>
-      <c r="F30" s="18"/>
-      <c r="G30" s="18" t="s">
+      <c r="F30" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="G30" s="17" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
         <v>40</v>
       </c>
@@ -1182,12 +1258,14 @@
       <c r="C31" s="7"/>
       <c r="D31" s="7"/>
       <c r="E31" s="7"/>
-      <c r="F31" s="18"/>
-      <c r="G31" s="18" t="s">
+      <c r="F31" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="G31" s="17" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
         <v>42</v>
       </c>
@@ -1197,12 +1275,14 @@
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>
       <c r="E32" s="7"/>
-      <c r="F32" s="18"/>
-      <c r="G32" s="18" t="s">
+      <c r="F32" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="G32" s="17" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
         <v>33</v>
       </c>
@@ -1212,12 +1292,14 @@
       <c r="C33" s="7"/>
       <c r="D33" s="7"/>
       <c r="E33" s="7"/>
-      <c r="F33" s="18"/>
-      <c r="G33" s="18" t="s">
+      <c r="F33" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="G33" s="17" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
         <v>44</v>
       </c>
@@ -1227,12 +1309,14 @@
       <c r="C34" s="7"/>
       <c r="D34" s="7"/>
       <c r="E34" s="7"/>
-      <c r="F34" s="18"/>
-      <c r="G34" s="18" t="s">
+      <c r="F34" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="G34" s="17" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
         <v>45</v>
       </c>
@@ -1242,12 +1326,14 @@
       <c r="C35" s="7"/>
       <c r="D35" s="7"/>
       <c r="E35" s="7"/>
-      <c r="F35" s="18"/>
-      <c r="G35" s="18" t="s">
+      <c r="F35" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="G35" s="17" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
         <v>46</v>
       </c>
@@ -1257,12 +1343,14 @@
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
-      <c r="F36" s="18"/>
-      <c r="G36" s="18" t="s">
+      <c r="F36" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="G36" s="17" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="45">
+    <row r="37" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
         <v>30</v>
       </c>
@@ -1272,10 +1360,12 @@
       <c r="C37" s="7"/>
       <c r="D37" s="7"/>
       <c r="E37" s="7"/>
-      <c r="F37" s="18"/>
-      <c r="G37" s="18"/>
-    </row>
-    <row r="38" spans="1:7">
+      <c r="F37" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="G37" s="17"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
         <v>82</v>
       </c>
@@ -1285,10 +1375,12 @@
       <c r="C38" s="7"/>
       <c r="D38" s="7"/>
       <c r="E38" s="7"/>
-      <c r="F38" s="18"/>
-      <c r="G38" s="18"/>
-    </row>
-    <row r="39" spans="1:7">
+      <c r="F38" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="G38" s="17"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
         <v>79</v>
       </c>
@@ -1298,10 +1390,12 @@
       <c r="C39" s="7"/>
       <c r="D39" s="7"/>
       <c r="E39" s="7"/>
-      <c r="F39" s="18"/>
-      <c r="G39" s="18"/>
-    </row>
-    <row r="40" spans="1:7">
+      <c r="F39" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="G39" s="17"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
         <v>80</v>
       </c>
@@ -1311,10 +1405,12 @@
       <c r="C40" s="7"/>
       <c r="D40" s="7"/>
       <c r="E40" s="7"/>
-      <c r="F40" s="18"/>
-      <c r="G40" s="18"/>
-    </row>
-    <row r="41" spans="1:7">
+      <c r="F40" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="G40" s="17"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
         <v>54</v>
       </c>
@@ -1324,12 +1420,14 @@
       <c r="C41" s="9"/>
       <c r="D41" s="9"/>
       <c r="E41" s="9"/>
-      <c r="F41" s="18"/>
-      <c r="G41" s="18" t="s">
+      <c r="F41" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="G41" s="17" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="9" t="s">
         <v>56</v>
       </c>
@@ -1339,12 +1437,14 @@
       <c r="C42" s="9"/>
       <c r="D42" s="9"/>
       <c r="E42" s="9"/>
-      <c r="F42" s="18"/>
-      <c r="G42" s="18" t="s">
+      <c r="F42" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="G42" s="17" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="9" t="s">
         <v>58</v>
       </c>
@@ -1354,10 +1454,12 @@
       <c r="C43" s="9"/>
       <c r="D43" s="9"/>
       <c r="E43" s="9"/>
-      <c r="F43" s="18"/>
-      <c r="G43" s="18"/>
-    </row>
-    <row r="44" spans="1:7">
+      <c r="F43" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="G43" s="17"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="s">
         <v>60</v>
       </c>
@@ -1367,12 +1469,14 @@
       <c r="C44" s="9"/>
       <c r="D44" s="9"/>
       <c r="E44" s="9"/>
-      <c r="F44" s="18"/>
-      <c r="G44" s="18" t="s">
+      <c r="F44" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="G44" s="17" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="9" t="s">
         <v>84</v>
       </c>
@@ -1382,8 +1486,10 @@
       <c r="C45" s="9"/>
       <c r="D45" s="9"/>
       <c r="E45" s="9"/>
-      <c r="F45" s="18"/>
-      <c r="G45" s="18"/>
+      <c r="F45" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="G45" s="17"/>
     </row>
   </sheetData>
   <autoFilter ref="A5:G45"/>
@@ -1393,24 +1499,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
actualice planilla y modifique el login.
</commit_message>
<xml_diff>
--- a/ProjectItems/Tareas iCatalog.xlsx
+++ b/ProjectItems/Tareas iCatalog.xlsx
@@ -420,7 +420,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -461,6 +461,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -770,10 +773,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -922,8 +926,8 @@
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
-      <c r="F11" s="16" t="s">
-        <v>88</v>
+      <c r="F11" s="20" t="s">
+        <v>87</v>
       </c>
       <c r="G11" s="17" t="s">
         <v>92</v>
@@ -980,7 +984,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>67</v>
       </c>
@@ -997,7 +1001,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>21</v>
       </c>
@@ -1031,7 +1035,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>35</v>
       </c>
@@ -1048,7 +1052,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>74</v>
       </c>
@@ -1065,7 +1069,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>69</v>
       </c>
@@ -1082,7 +1086,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>47</v>
       </c>
@@ -1099,7 +1103,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>75</v>
       </c>
@@ -1116,7 +1120,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>77</v>
       </c>
@@ -1133,7 +1137,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>81</v>
       </c>
@@ -1148,7 +1152,7 @@
       </c>
       <c r="G24" s="17"/>
     </row>
-    <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>71</v>
       </c>
@@ -1248,7 +1252,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
         <v>40</v>
       </c>
@@ -1265,7 +1269,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
         <v>42</v>
       </c>
@@ -1282,7 +1286,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
         <v>33</v>
       </c>
@@ -1299,7 +1303,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
         <v>44</v>
       </c>
@@ -1316,7 +1320,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
         <v>45</v>
       </c>
@@ -1333,7 +1337,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
         <v>46</v>
       </c>
@@ -1350,7 +1354,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" ht="30.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
         <v>30</v>
       </c>
@@ -1365,7 +1369,7 @@
       </c>
       <c r="G37" s="17"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
         <v>82</v>
       </c>
@@ -1380,7 +1384,7 @@
       </c>
       <c r="G38" s="17"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
         <v>79</v>
       </c>
@@ -1395,7 +1399,7 @@
       </c>
       <c r="G39" s="17"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
         <v>80</v>
       </c>
@@ -1410,7 +1414,7 @@
       </c>
       <c r="G40" s="17"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
         <v>54</v>
       </c>
@@ -1444,7 +1448,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="9" t="s">
         <v>58</v>
       </c>
@@ -1459,7 +1463,7 @@
       </c>
       <c r="G43" s="17"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="s">
         <v>60</v>
       </c>
@@ -1476,7 +1480,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="9" t="s">
         <v>84</v>
       </c>
@@ -1492,7 +1496,13 @@
       <c r="G45" s="17"/>
     </row>
   </sheetData>
-  <autoFilter ref="A5:G45"/>
+  <autoFilter ref="A5:G45">
+    <filterColumn colId="6">
+      <filters>
+        <filter val="Sebas"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Se avanza con Productos
</commit_message>
<xml_diff>
--- a/ProjectItems/Tareas iCatalog.xlsx
+++ b/ProjectItems/Tareas iCatalog.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="75" windowWidth="20115" windowHeight="7995"/>
@@ -315,8 +315,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -468,8 +468,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Heading 2" xfId="1" builtinId="17"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Título 2" xfId="1" builtinId="17"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -487,7 +487,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -561,7 +561,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -596,7 +595,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -772,15 +770,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="45" customWidth="1"/>
     <col min="2" max="2" width="59" customWidth="1"/>
@@ -789,26 +786,26 @@
     <col min="7" max="7" width="12.7109375" style="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="3" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="11"/>
       <c r="B4" s="11"/>
     </row>
-    <row r="5" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" ht="18" thickBot="1">
       <c r="A5" s="12" t="s">
         <v>0</v>
       </c>
@@ -831,7 +828,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="15.75" thickTop="1">
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
@@ -848,7 +845,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
@@ -865,7 +862,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8" s="4" t="s">
         <v>9</v>
       </c>
@@ -882,7 +879,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" s="4" t="s">
         <v>11</v>
       </c>
@@ -899,7 +896,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10" s="4" t="s">
         <v>13</v>
       </c>
@@ -916,7 +913,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="30">
       <c r="A11" s="4" t="s">
         <v>18</v>
       </c>
@@ -933,7 +930,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12" s="4" t="s">
         <v>65</v>
       </c>
@@ -950,7 +947,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13" s="4" t="s">
         <v>16</v>
       </c>
@@ -967,7 +964,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7">
       <c r="A14" s="4" t="s">
         <v>19</v>
       </c>
@@ -984,7 +981,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="15" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7">
       <c r="A15" s="4" t="s">
         <v>67</v>
       </c>
@@ -1001,7 +998,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="16" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7">
       <c r="A16" s="4" t="s">
         <v>21</v>
       </c>
@@ -1018,7 +1015,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="30">
       <c r="A17" s="4" t="s">
         <v>23</v>
       </c>
@@ -1035,7 +1032,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="30">
       <c r="A18" s="4" t="s">
         <v>35</v>
       </c>
@@ -1052,7 +1049,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="19" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7">
       <c r="A19" s="4" t="s">
         <v>74</v>
       </c>
@@ -1069,7 +1066,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="20" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7">
       <c r="A20" s="4" t="s">
         <v>69</v>
       </c>
@@ -1086,7 +1083,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="30">
       <c r="A21" s="4" t="s">
         <v>47</v>
       </c>
@@ -1103,7 +1100,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="22" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7">
       <c r="A22" s="4" t="s">
         <v>75</v>
       </c>
@@ -1120,7 +1117,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="23" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7">
       <c r="A23" s="4" t="s">
         <v>77</v>
       </c>
@@ -1137,7 +1134,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="30">
       <c r="A24" s="4" t="s">
         <v>81</v>
       </c>
@@ -1152,7 +1149,7 @@
       </c>
       <c r="G24" s="17"/>
     </row>
-    <row r="25" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="30">
       <c r="A25" s="4" t="s">
         <v>71</v>
       </c>
@@ -1167,7 +1164,7 @@
       </c>
       <c r="G25" s="17"/>
     </row>
-    <row r="26" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="30">
       <c r="A26" s="4" t="s">
         <v>26</v>
       </c>
@@ -1184,7 +1181,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="30">
       <c r="A27" s="7" t="s">
         <v>28</v>
       </c>
@@ -1201,7 +1198,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="30">
       <c r="A28" s="8" t="s">
         <v>38</v>
       </c>
@@ -1218,7 +1215,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7">
       <c r="A29" s="7" t="s">
         <v>31</v>
       </c>
@@ -1235,7 +1232,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" ht="45.75" customHeight="1">
       <c r="A30" s="8" t="s">
         <v>43</v>
       </c>
@@ -1252,7 +1249,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="31" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7">
       <c r="A31" s="7" t="s">
         <v>40</v>
       </c>
@@ -1269,7 +1266,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="32" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7">
       <c r="A32" s="7" t="s">
         <v>42</v>
       </c>
@@ -1286,7 +1283,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="33" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7">
       <c r="A33" s="7" t="s">
         <v>33</v>
       </c>
@@ -1296,14 +1293,14 @@
       <c r="C33" s="7"/>
       <c r="D33" s="7"/>
       <c r="E33" s="7"/>
-      <c r="F33" s="18" t="s">
-        <v>95</v>
+      <c r="F33" s="15" t="s">
+        <v>87</v>
       </c>
       <c r="G33" s="17" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="34" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7">
       <c r="A34" s="8" t="s">
         <v>44</v>
       </c>
@@ -1313,14 +1310,14 @@
       <c r="C34" s="7"/>
       <c r="D34" s="7"/>
       <c r="E34" s="7"/>
-      <c r="F34" s="18" t="s">
-        <v>95</v>
+      <c r="F34" s="15" t="s">
+        <v>87</v>
       </c>
       <c r="G34" s="17" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="35" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7">
       <c r="A35" s="7" t="s">
         <v>45</v>
       </c>
@@ -1337,7 +1334,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="36" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7">
       <c r="A36" s="7" t="s">
         <v>46</v>
       </c>
@@ -1354,7 +1351,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="30.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" ht="30.75" customHeight="1">
       <c r="A37" s="7" t="s">
         <v>30</v>
       </c>
@@ -1369,7 +1366,7 @@
       </c>
       <c r="G37" s="17"/>
     </row>
-    <row r="38" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7">
       <c r="A38" s="7" t="s">
         <v>82</v>
       </c>
@@ -1384,7 +1381,7 @@
       </c>
       <c r="G38" s="17"/>
     </row>
-    <row r="39" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7">
       <c r="A39" s="7" t="s">
         <v>79</v>
       </c>
@@ -1399,7 +1396,7 @@
       </c>
       <c r="G39" s="17"/>
     </row>
-    <row r="40" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7">
       <c r="A40" s="7" t="s">
         <v>80</v>
       </c>
@@ -1414,7 +1411,7 @@
       </c>
       <c r="G40" s="17"/>
     </row>
-    <row r="41" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7">
       <c r="A41" s="9" t="s">
         <v>54</v>
       </c>
@@ -1431,7 +1428,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7">
       <c r="A42" s="9" t="s">
         <v>56</v>
       </c>
@@ -1448,7 +1445,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="43" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7">
       <c r="A43" s="9" t="s">
         <v>58</v>
       </c>
@@ -1463,7 +1460,7 @@
       </c>
       <c r="G43" s="17"/>
     </row>
-    <row r="44" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7">
       <c r="A44" s="9" t="s">
         <v>60</v>
       </c>
@@ -1480,7 +1477,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="45" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7">
       <c r="A45" s="9" t="s">
         <v>84</v>
       </c>
@@ -1497,11 +1494,7 @@
     </row>
   </sheetData>
   <autoFilter ref="A5:G45">
-    <filterColumn colId="6">
-      <filters>
-        <filter val="Sebas"/>
-      </filters>
-    </filterColumn>
+    <filterColumn colId="6"/>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1509,24 +1502,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Agregando las categorias al abm de productos
</commit_message>
<xml_diff>
--- a/ProjectItems/Tareas iCatalog.xlsx
+++ b/ProjectItems/Tareas iCatalog.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="20115" windowHeight="7995"/>
+    <workbookView xWindow="120" yWindow="75" windowWidth="19440" windowHeight="7995"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -315,8 +315,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -468,8 +468,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
+    <cellStyle name="Heading 2" xfId="1" builtinId="17"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Título 2" xfId="1" builtinId="17"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -487,7 +487,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -561,6 +561,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -595,6 +596,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -770,14 +772,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="45" customWidth="1"/>
     <col min="2" max="2" width="59" customWidth="1"/>
@@ -786,26 +788,26 @@
     <col min="7" max="7" width="12.7109375" style="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="11"/>
       <c r="B4" s="11"/>
     </row>
-    <row r="5" spans="1:7" ht="18" thickBot="1">
+    <row r="5" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="12" t="s">
         <v>0</v>
       </c>
@@ -828,7 +830,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" thickTop="1">
+    <row r="6" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
@@ -845,7 +847,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
@@ -862,7 +864,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>9</v>
       </c>
@@ -879,7 +881,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>11</v>
       </c>
@@ -896,7 +898,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>13</v>
       </c>
@@ -913,7 +915,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="30">
+    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>18</v>
       </c>
@@ -930,7 +932,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>65</v>
       </c>
@@ -947,7 +949,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>16</v>
       </c>
@@ -964,7 +966,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>19</v>
       </c>
@@ -981,7 +983,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>67</v>
       </c>
@@ -998,7 +1000,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>21</v>
       </c>
@@ -1015,7 +1017,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="30">
+    <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>23</v>
       </c>
@@ -1032,7 +1034,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="30">
+    <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>35</v>
       </c>
@@ -1049,7 +1051,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>74</v>
       </c>
@@ -1066,7 +1068,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>69</v>
       </c>
@@ -1083,7 +1085,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="30">
+    <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>47</v>
       </c>
@@ -1100,7 +1102,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>75</v>
       </c>
@@ -1117,7 +1119,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>77</v>
       </c>
@@ -1134,7 +1136,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="30">
+    <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>81</v>
       </c>
@@ -1149,7 +1151,7 @@
       </c>
       <c r="G24" s="17"/>
     </row>
-    <row r="25" spans="1:7" ht="30">
+    <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>71</v>
       </c>
@@ -1164,7 +1166,7 @@
       </c>
       <c r="G25" s="17"/>
     </row>
-    <row r="26" spans="1:7" ht="30">
+    <row r="26" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>26</v>
       </c>
@@ -1181,7 +1183,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="30">
+    <row r="27" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>28</v>
       </c>
@@ -1198,7 +1200,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="30">
+    <row r="28" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
         <v>38</v>
       </c>
@@ -1215,7 +1217,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
         <v>31</v>
       </c>
@@ -1225,14 +1227,14 @@
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
       <c r="E29" s="7"/>
-      <c r="F29" s="18" t="s">
-        <v>95</v>
+      <c r="F29" s="15" t="s">
+        <v>87</v>
       </c>
       <c r="G29" s="17" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="45.75" customHeight="1">
+    <row r="30" spans="1:7" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
         <v>43</v>
       </c>
@@ -1242,14 +1244,14 @@
       <c r="C30" s="7"/>
       <c r="D30" s="7"/>
       <c r="E30" s="7"/>
-      <c r="F30" s="18" t="s">
-        <v>95</v>
+      <c r="F30" s="20" t="s">
+        <v>87</v>
       </c>
       <c r="G30" s="17" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
         <v>40</v>
       </c>
@@ -1266,7 +1268,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
         <v>42</v>
       </c>
@@ -1283,7 +1285,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
         <v>33</v>
       </c>
@@ -1300,7 +1302,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
         <v>44</v>
       </c>
@@ -1317,7 +1319,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
         <v>45</v>
       </c>
@@ -1334,7 +1336,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
         <v>46</v>
       </c>
@@ -1351,7 +1353,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="30.75" customHeight="1">
+    <row r="37" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
         <v>30</v>
       </c>
@@ -1366,7 +1368,7 @@
       </c>
       <c r="G37" s="17"/>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
         <v>82</v>
       </c>
@@ -1381,7 +1383,7 @@
       </c>
       <c r="G38" s="17"/>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
         <v>79</v>
       </c>
@@ -1396,7 +1398,7 @@
       </c>
       <c r="G39" s="17"/>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
         <v>80</v>
       </c>
@@ -1411,7 +1413,7 @@
       </c>
       <c r="G40" s="17"/>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
         <v>54</v>
       </c>
@@ -1428,7 +1430,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="9" t="s">
         <v>56</v>
       </c>
@@ -1445,7 +1447,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="9" t="s">
         <v>58</v>
       </c>
@@ -1460,7 +1462,7 @@
       </c>
       <c r="G43" s="17"/>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="s">
         <v>60</v>
       </c>
@@ -1477,7 +1479,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="9" t="s">
         <v>84</v>
       </c>
@@ -1493,33 +1495,31 @@
       <c r="G45" s="17"/>
     </row>
   </sheetData>
-  <autoFilter ref="A5:G45">
-    <filterColumn colId="6"/>
-  </autoFilter>
+  <autoFilter ref="A5:G45"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Starting again with iCatalog
</commit_message>
<xml_diff>
--- a/ProjectItems/Tareas iCatalog.xlsx
+++ b/ProjectItems/Tareas iCatalog.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="75" windowWidth="19440" windowHeight="7995"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="93">
   <si>
     <t>Tarea</t>
   </si>
@@ -288,22 +288,10 @@
     <t>in progress</t>
   </si>
   <si>
-    <t>Pablo</t>
-  </si>
-  <si>
-    <t>Penacho</t>
-  </si>
-  <si>
-    <t>Chiquito</t>
-  </si>
-  <si>
     <t>Sebas</t>
   </si>
   <si>
     <t>Persona</t>
-  </si>
-  <si>
-    <t>Sebas/Pablo</t>
   </si>
   <si>
     <t>pending</t>
@@ -468,8 +456,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Heading 2" xfId="1" builtinId="17"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Título 2" xfId="1" builtinId="17"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -487,7 +475,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -775,11 +763,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G42" sqref="G42"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="45" customWidth="1"/>
     <col min="2" max="2" width="59" customWidth="1"/>
@@ -827,7 +815,7 @@
         <v>86</v>
       </c>
       <c r="G5" s="13" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -844,7 +832,7 @@
         <v>87</v>
       </c>
       <c r="G6" s="17" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -861,7 +849,7 @@
         <v>87</v>
       </c>
       <c r="G7" s="17" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -878,7 +866,7 @@
         <v>87</v>
       </c>
       <c r="G8" s="17" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -895,7 +883,7 @@
         <v>87</v>
       </c>
       <c r="G9" s="17" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -912,7 +900,7 @@
         <v>87</v>
       </c>
       <c r="G10" s="17" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -929,7 +917,7 @@
         <v>87</v>
       </c>
       <c r="G11" s="17" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -946,7 +934,7 @@
         <v>87</v>
       </c>
       <c r="G12" s="17" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -963,7 +951,7 @@
         <v>87</v>
       </c>
       <c r="G13" s="17" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -980,7 +968,7 @@
         <v>87</v>
       </c>
       <c r="G14" s="17" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -997,7 +985,7 @@
         <v>87</v>
       </c>
       <c r="G15" s="17" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -1014,7 +1002,7 @@
         <v>87</v>
       </c>
       <c r="G16" s="17" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1028,10 +1016,10 @@
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
       <c r="F17" s="18" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="G17" s="17" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1045,7 +1033,7 @@
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
       <c r="F18" s="18" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="G18" s="17" t="s">
         <v>89</v>
@@ -1062,7 +1050,7 @@
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
       <c r="F19" s="18" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="G19" s="17" t="s">
         <v>89</v>
@@ -1079,7 +1067,7 @@
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
       <c r="F20" s="18" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="G20" s="17" t="s">
         <v>89</v>
@@ -1096,7 +1084,7 @@
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
       <c r="F21" s="18" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="G21" s="17" t="s">
         <v>89</v>
@@ -1113,7 +1101,7 @@
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
       <c r="F22" s="18" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="G22" s="17" t="s">
         <v>89</v>
@@ -1130,7 +1118,7 @@
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
       <c r="F23" s="18" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="G23" s="17" t="s">
         <v>89</v>
@@ -1147,9 +1135,11 @@
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
       <c r="F24" s="19" t="s">
-        <v>96</v>
-      </c>
-      <c r="G24" s="17"/>
+        <v>92</v>
+      </c>
+      <c r="G24" s="17" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
@@ -1162,9 +1152,11 @@
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
       <c r="F25" s="19" t="s">
-        <v>96</v>
-      </c>
-      <c r="G25" s="17"/>
+        <v>92</v>
+      </c>
+      <c r="G25" s="17" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="26" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
@@ -1180,7 +1172,7 @@
         <v>88</v>
       </c>
       <c r="G26" s="17" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1194,10 +1186,10 @@
       <c r="D27" s="7"/>
       <c r="E27" s="7"/>
       <c r="F27" s="18" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="G27" s="17" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1211,10 +1203,10 @@
       <c r="D28" s="7"/>
       <c r="E28" s="7"/>
       <c r="F28" s="18" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="G28" s="17" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -1231,7 +1223,7 @@
         <v>87</v>
       </c>
       <c r="G29" s="17" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1248,7 +1240,7 @@
         <v>87</v>
       </c>
       <c r="G30" s="17" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -1262,10 +1254,10 @@
       <c r="D31" s="7"/>
       <c r="E31" s="7"/>
       <c r="F31" s="18" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="G31" s="17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -1279,10 +1271,10 @@
       <c r="D32" s="7"/>
       <c r="E32" s="7"/>
       <c r="F32" s="18" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="G32" s="17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -1299,7 +1291,7 @@
         <v>87</v>
       </c>
       <c r="G33" s="17" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -1316,7 +1308,7 @@
         <v>87</v>
       </c>
       <c r="G34" s="17" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -1330,10 +1322,10 @@
       <c r="D35" s="7"/>
       <c r="E35" s="7"/>
       <c r="F35" s="18" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="G35" s="17" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -1347,10 +1339,10 @@
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="F36" s="18" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="G36" s="17" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1364,9 +1356,11 @@
       <c r="D37" s="7"/>
       <c r="E37" s="7"/>
       <c r="F37" s="19" t="s">
-        <v>96</v>
-      </c>
-      <c r="G37" s="17"/>
+        <v>92</v>
+      </c>
+      <c r="G37" s="17" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
@@ -1379,9 +1373,11 @@
       <c r="D38" s="7"/>
       <c r="E38" s="7"/>
       <c r="F38" s="19" t="s">
-        <v>96</v>
-      </c>
-      <c r="G38" s="17"/>
+        <v>92</v>
+      </c>
+      <c r="G38" s="17" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
@@ -1394,9 +1390,11 @@
       <c r="D39" s="7"/>
       <c r="E39" s="7"/>
       <c r="F39" s="19" t="s">
-        <v>96</v>
-      </c>
-      <c r="G39" s="17"/>
+        <v>92</v>
+      </c>
+      <c r="G39" s="17" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
@@ -1409,9 +1407,11 @@
       <c r="D40" s="7"/>
       <c r="E40" s="7"/>
       <c r="F40" s="19" t="s">
-        <v>96</v>
-      </c>
-      <c r="G40" s="17"/>
+        <v>92</v>
+      </c>
+      <c r="G40" s="17" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
@@ -1424,10 +1424,10 @@
       <c r="D41" s="9"/>
       <c r="E41" s="9"/>
       <c r="F41" s="18" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="G41" s="17" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
@@ -1444,7 +1444,7 @@
         <v>88</v>
       </c>
       <c r="G42" s="17" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -1458,9 +1458,11 @@
       <c r="D43" s="9"/>
       <c r="E43" s="9"/>
       <c r="F43" s="19" t="s">
-        <v>96</v>
-      </c>
-      <c r="G43" s="17"/>
+        <v>92</v>
+      </c>
+      <c r="G43" s="17" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="s">
@@ -1473,10 +1475,10 @@
       <c r="D44" s="9"/>
       <c r="E44" s="9"/>
       <c r="F44" s="18" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="G44" s="17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
@@ -1490,9 +1492,11 @@
       <c r="D45" s="9"/>
       <c r="E45" s="9"/>
       <c r="F45" s="19" t="s">
-        <v>96</v>
-      </c>
-      <c r="G45" s="17"/>
+        <v>92</v>
+      </c>
+      <c r="G45" s="17" t="s">
+        <v>89</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A5:G45"/>
@@ -1507,7 +1511,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1519,7 +1523,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>